<commit_message>
Added frozen headers for printing
</commit_message>
<xml_diff>
--- a/CoC_Spread.xlsx
+++ b/CoC_Spread.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwiltberger\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwiltberger\Documents\ClashOfClans\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$2</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1119,8 +1122,9 @@
   </sheetPr>
   <dimension ref="A1:AD139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J112" workbookViewId="0">
-      <selection activeCell="AB123" sqref="AB123"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9964,12 +9968,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
@@ -9977,6 +9975,12 @@
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="46" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed incorrect date upgrades for Barbarian King and Archer Queen
</commit_message>
<xml_diff>
--- a/CoC_Spread.xlsx
+++ b/CoC_Spread.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="100">
   <si>
     <t>Town Hall</t>
   </si>
@@ -306,9 +306,6 @@
   </si>
   <si>
     <t>5.5 days</t>
-  </si>
-  <si>
-    <t>6.5 days</t>
   </si>
   <si>
     <t>15min</t>
@@ -1122,9 +1119,9 @@
   </sheetPr>
   <dimension ref="A1:AD139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,7 +1254,7 @@
         <v>25000</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K3" s="16">
         <v>150000</v>
@@ -1327,7 +1324,7 @@
         <v>800000</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I4" s="11">
         <v>1800000</v>
@@ -1393,7 +1390,7 @@
         <v>270000</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K5" s="13">
         <v>500000</v>
@@ -1443,7 +1440,7 @@
         <v>200000</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E6" s="15">
         <v>400000</v>
@@ -1542,7 +1539,7 @@
         <v>150000</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I8" s="13">
         <v>500000</v>
@@ -1664,7 +1661,7 @@
         <v>100000</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G10" s="15">
         <v>250000</v>
@@ -1788,7 +1785,7 @@
         <v>100000</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G12" s="15">
         <v>250000</v>
@@ -1846,7 +1843,7 @@
         <v>150000</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G13" s="15">
         <v>450000</v>
@@ -1906,7 +1903,7 @@
         <v>150000</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G14" s="15">
         <v>450000</v>
@@ -2440,7 +2437,7 @@
         <v>200000</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G24" s="16">
         <v>500000</v>
@@ -2500,7 +2497,7 @@
         <v>300000</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G25" s="15">
         <v>600000</v>
@@ -2759,67 +2756,67 @@
         <v>15000</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="I30" s="13">
         <v>17500</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="K30" s="13">
         <v>20000</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="M30" s="11">
         <v>22500</v>
       </c>
       <c r="N30" s="11" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="O30" s="11">
         <v>25000</v>
       </c>
       <c r="P30" s="11" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="Q30" s="11">
         <v>30000</v>
       </c>
       <c r="R30" s="11" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="S30" s="11">
         <v>35000</v>
       </c>
       <c r="T30" s="11" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="U30" s="11">
         <v>40000</v>
       </c>
       <c r="V30" s="11" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="W30" s="9">
         <v>45000</v>
       </c>
       <c r="X30" s="9" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="Y30" s="9">
         <v>50000</v>
       </c>
       <c r="Z30" s="9" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AA30" s="9">
         <v>55000</v>
       </c>
       <c r="AB30" s="9" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="AC30" s="4" t="s">
         <v>63</v>
@@ -2849,67 +2846,67 @@
         <v>25000</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="I31" s="9">
         <v>27500</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="K31" s="9">
         <v>30000</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="M31" s="9">
         <v>32500</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="O31" s="9">
         <v>35000</v>
       </c>
       <c r="P31" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="Q31" s="9">
         <v>40000</v>
       </c>
       <c r="R31" s="9" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="S31" s="9">
         <v>45000</v>
       </c>
       <c r="T31" s="9" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="U31" s="9">
         <v>50000</v>
       </c>
       <c r="V31" s="9" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="W31" s="9">
         <v>55000</v>
       </c>
       <c r="X31" s="9" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="Y31" s="9">
         <v>60000</v>
       </c>
       <c r="Z31" s="9" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AA31" s="9">
         <v>65000</v>
       </c>
       <c r="AB31" s="9" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="AC31" s="4" t="s">
         <v>63</v>
@@ -2966,7 +2963,7 @@
         <v>90000</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G33" s="16">
         <v>270000</v>
@@ -3034,7 +3031,7 @@
         <v>90000</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G34" s="13">
         <v>270000</v>
@@ -3102,7 +3099,7 @@
         <v>90000</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G35" s="11">
         <v>270000</v>
@@ -3170,7 +3167,7 @@
         <v>90000</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G36" s="9">
         <v>270000</v>
@@ -3225,7 +3222,7 @@
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
         <v>59</v>
@@ -3234,7 +3231,7 @@
         <v>500000</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E37" s="15">
         <v>750000</v>
@@ -3294,7 +3291,7 @@
         <v>1000</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E38" s="22">
         <v>2000</v>
@@ -3306,7 +3303,7 @@
         <v>5000</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I38" s="19">
         <v>20000</v>
@@ -3324,7 +3321,7 @@
         <v>180000</v>
       </c>
       <c r="N38" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O38" s="15">
         <v>360000</v>
@@ -3382,7 +3379,7 @@
         <v>1000</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E39" s="23">
         <v>2000</v>
@@ -3394,7 +3391,7 @@
         <v>5000</v>
       </c>
       <c r="H39" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I39" s="19">
         <v>20000</v>
@@ -3412,7 +3409,7 @@
         <v>180000</v>
       </c>
       <c r="N39" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O39" s="15">
         <v>360000</v>
@@ -3470,7 +3467,7 @@
         <v>1000</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E40" s="25">
         <v>2000</v>
@@ -3482,7 +3479,7 @@
         <v>5000</v>
       </c>
       <c r="H40" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I40" s="27">
         <v>20000</v>
@@ -3500,7 +3497,7 @@
         <v>180000</v>
       </c>
       <c r="N40" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O40" s="15">
         <v>360000</v>
@@ -3558,7 +3555,7 @@
         <v>1000</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E41" s="30">
         <v>2000</v>
@@ -3570,7 +3567,7 @@
         <v>5000</v>
       </c>
       <c r="H41" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I41" s="32">
         <v>20000</v>
@@ -3588,7 +3585,7 @@
         <v>180000</v>
       </c>
       <c r="N41" s="44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O41" s="17">
         <v>360000</v>
@@ -3646,7 +3643,7 @@
         <v>1000</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E42" s="33">
         <v>2000</v>
@@ -3658,7 +3655,7 @@
         <v>5000</v>
       </c>
       <c r="H42" s="34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I42" s="35">
         <v>20000</v>
@@ -3676,7 +3673,7 @@
         <v>180000</v>
       </c>
       <c r="N42" s="45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O42" s="36">
         <v>360000</v>
@@ -3734,7 +3731,7 @@
         <v>1000</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E43" s="38">
         <v>2000</v>
@@ -3746,7 +3743,7 @@
         <v>5000</v>
       </c>
       <c r="H43" s="39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I43" s="40">
         <v>20000</v>
@@ -3764,7 +3761,7 @@
         <v>180000</v>
       </c>
       <c r="N43" s="46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O43" s="41">
         <v>360000</v>
@@ -3822,7 +3819,7 @@
         <v>1000</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E44" s="28">
         <v>2000</v>
@@ -3834,7 +3831,7 @@
         <v>5000</v>
       </c>
       <c r="H44" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I44" s="18">
         <v>20000</v>
@@ -3852,7 +3849,7 @@
         <v>180000</v>
       </c>
       <c r="N44" s="47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O44" s="14">
         <v>360000</v>
@@ -3916,13 +3913,13 @@
         <v>1000</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G45" s="22">
         <v>4000</v>
       </c>
       <c r="H45" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I45" s="20">
         <v>16000</v>
@@ -3946,7 +3943,7 @@
         <v>200000</v>
       </c>
       <c r="P45" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q45" s="13">
         <v>400000</v>
@@ -4004,13 +4001,13 @@
         <v>1000</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G46" s="22">
         <v>4000</v>
       </c>
       <c r="H46" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I46" s="20">
         <v>16000</v>
@@ -4034,7 +4031,7 @@
         <v>200000</v>
       </c>
       <c r="P46" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q46" s="13">
         <v>400000</v>
@@ -4092,13 +4089,13 @@
         <v>1000</v>
       </c>
       <c r="F47" s="49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G47" s="50">
         <v>4000</v>
       </c>
       <c r="H47" s="50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I47" s="51">
         <v>16000</v>
@@ -4122,7 +4119,7 @@
         <v>200000</v>
       </c>
       <c r="P47" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q47" s="13">
         <v>400000</v>
@@ -4180,13 +4177,13 @@
         <v>1000</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G48" s="30">
         <v>4000</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I48" s="31">
         <v>16000</v>
@@ -4210,7 +4207,7 @@
         <v>200000</v>
       </c>
       <c r="P48" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q48" s="13">
         <v>400000</v>
@@ -4268,13 +4265,13 @@
         <v>1000</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G49" s="30">
         <v>4000</v>
       </c>
       <c r="H49" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I49" s="31">
         <v>16000</v>
@@ -4298,7 +4295,7 @@
         <v>200000</v>
       </c>
       <c r="P49" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q49" s="13">
         <v>400000</v>
@@ -4356,13 +4353,13 @@
         <v>1000</v>
       </c>
       <c r="F50" s="53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G50" s="28">
         <v>4000</v>
       </c>
       <c r="H50" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I50" s="29">
         <v>16000</v>
@@ -4386,7 +4383,7 @@
         <v>200000</v>
       </c>
       <c r="P50" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q50" s="12">
         <v>400000</v>
@@ -4438,7 +4435,7 @@
         <v>8000</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E51" s="19">
         <v>32000</v>
@@ -4450,7 +4447,7 @@
         <v>120000</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I51" s="15">
         <v>400000</v>
@@ -4506,7 +4503,7 @@
         <v>8000</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E52" s="54">
         <v>32000</v>
@@ -4518,7 +4515,7 @@
         <v>120000</v>
       </c>
       <c r="H52" s="55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I52" s="15">
         <v>400000</v>
@@ -4574,7 +4571,7 @@
         <v>8000</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E53" s="32">
         <v>32000</v>
@@ -4586,7 +4583,7 @@
         <v>120000</v>
       </c>
       <c r="H53" s="44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I53" s="17">
         <v>400000</v>
@@ -4642,7 +4639,7 @@
         <v>8000</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E54" s="35">
         <v>32000</v>
@@ -4654,7 +4651,7 @@
         <v>120000</v>
       </c>
       <c r="H54" s="45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I54" s="36">
         <v>400000</v>
@@ -4716,7 +4713,7 @@
         <v>360000</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G55" s="15">
         <v>720000</v>
@@ -4784,7 +4781,7 @@
         <v>360000</v>
       </c>
       <c r="F56" s="55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G56" s="15">
         <v>720000</v>
@@ -4852,7 +4849,7 @@
         <v>360000</v>
       </c>
       <c r="F57" s="45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G57" s="36">
         <v>720000</v>
@@ -4920,7 +4917,7 @@
         <v>360000</v>
       </c>
       <c r="F58" s="46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G58" s="41">
         <v>720000</v>
@@ -4982,7 +4979,7 @@
         <v>1000000</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E59" s="13">
         <v>1250000</v>
@@ -5050,7 +5047,7 @@
         <v>1000000</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E60" s="13">
         <v>1250000</v>
@@ -5118,7 +5115,7 @@
         <v>1000000</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E61" s="37">
         <v>1250000</v>
@@ -5186,7 +5183,7 @@
         <v>1000000</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E62" s="12">
         <v>1250000</v>
@@ -5637,7 +5634,7 @@
         <v>1500000</v>
       </c>
       <c r="J70" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
@@ -5689,7 +5686,7 @@
         <v>1500000</v>
       </c>
       <c r="J71" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
@@ -5741,7 +5738,7 @@
         <v>1500000</v>
       </c>
       <c r="J72" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K72" s="4"/>
       <c r="L72" s="4"/>
@@ -5793,7 +5790,7 @@
         <v>1500000</v>
       </c>
       <c r="J73" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K73" s="4"/>
       <c r="L73" s="4"/>
@@ -5845,7 +5842,7 @@
         <v>1500000</v>
       </c>
       <c r="J74" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
@@ -5885,7 +5882,7 @@
         <v>1000</v>
       </c>
       <c r="F75" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G75" s="16">
         <v>10000</v>
@@ -5897,13 +5894,13 @@
         <v>100000</v>
       </c>
       <c r="J75" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K75" s="11">
         <v>1000000</v>
       </c>
       <c r="L75" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M75" s="9">
         <v>1500000</v>
@@ -5945,7 +5942,7 @@
         <v>1000</v>
       </c>
       <c r="F76" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G76" s="16">
         <v>10000</v>
@@ -5957,13 +5954,13 @@
         <v>100000</v>
       </c>
       <c r="J76" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K76" s="11">
         <v>1000000</v>
       </c>
       <c r="L76" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M76" s="9">
         <v>1500000</v>
@@ -6005,7 +6002,7 @@
         <v>1000</v>
       </c>
       <c r="F77" s="51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G77" s="16">
         <v>10000</v>
@@ -6017,13 +6014,13 @@
         <v>100000</v>
       </c>
       <c r="J77" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K77" s="11">
         <v>1000000</v>
       </c>
       <c r="L77" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M77" s="9">
         <v>1500000</v>
@@ -6065,7 +6062,7 @@
         <v>1000</v>
       </c>
       <c r="F78" s="51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G78" s="16">
         <v>10000</v>
@@ -6077,13 +6074,13 @@
         <v>100000</v>
       </c>
       <c r="J78" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K78" s="11">
         <v>1000000</v>
       </c>
       <c r="L78" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M78" s="9">
         <v>1500000</v>
@@ -6125,7 +6122,7 @@
         <v>1000</v>
       </c>
       <c r="F79" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G79" s="44">
         <v>10000</v>
@@ -6137,13 +6134,13 @@
         <v>100000</v>
       </c>
       <c r="J79" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K79" s="11">
         <v>1000000</v>
       </c>
       <c r="L79" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M79" s="9">
         <v>1500000</v>
@@ -6185,7 +6182,7 @@
         <v>1000</v>
       </c>
       <c r="F80" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G80" s="44">
         <v>10000</v>
@@ -6197,13 +6194,13 @@
         <v>100000</v>
       </c>
       <c r="J80" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K80" s="11">
         <v>1000000</v>
       </c>
       <c r="L80" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M80" s="9">
         <v>1500000</v>
@@ -6251,7 +6248,7 @@
         <v>750000</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I81" s="7">
         <v>2500000</v>
@@ -6303,7 +6300,7 @@
         <v>750000</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I82" s="7">
         <v>2500000</v>
@@ -6355,7 +6352,7 @@
         <v>750000</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I83" s="7">
         <v>2500000</v>
@@ -6407,7 +6404,7 @@
         <v>750000</v>
       </c>
       <c r="H84" s="43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I84" s="7">
         <v>2500000</v>
@@ -6459,7 +6456,7 @@
         <v>750000</v>
       </c>
       <c r="H85" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I85" s="7">
         <v>2500000</v>
@@ -6505,7 +6502,7 @@
         <v>2000000</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G86" s="7">
         <v>4000000</v>
@@ -6553,7 +6550,7 @@
         <v>2000000</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G87" s="7">
         <v>4000000</v>
@@ -6601,7 +6598,7 @@
         <v>2000000</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G88" s="7">
         <v>4000000</v>
@@ -6649,7 +6646,7 @@
         <v>2000000</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G89" s="7">
         <v>4000000</v>
@@ -6697,7 +6694,7 @@
         <v>2000000</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G90" s="7">
         <v>4000000</v>
@@ -6751,7 +6748,7 @@
         <v>1300000</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I91" s="4"/>
       <c r="J91" s="4"/>
@@ -6799,7 +6796,7 @@
         <v>1300000</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I92" s="4"/>
       <c r="J92" s="4"/>
@@ -6847,7 +6844,7 @@
         <v>1300000</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I93" s="4"/>
       <c r="J93" s="4"/>
@@ -7174,13 +7171,13 @@
         <v>100000</v>
       </c>
       <c r="J101" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K101" s="16">
         <v>250000</v>
       </c>
       <c r="L101" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M101" s="15">
         <v>750000</v>
@@ -7242,13 +7239,13 @@
         <v>100000</v>
       </c>
       <c r="J102" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K102" s="16">
         <v>250000</v>
       </c>
       <c r="L102" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M102" s="15">
         <v>750000</v>
@@ -7310,13 +7307,13 @@
         <v>100000</v>
       </c>
       <c r="J103" s="52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K103" s="16">
         <v>250000</v>
       </c>
       <c r="L103" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M103" s="15">
         <v>750000</v>
@@ -7378,13 +7375,13 @@
         <v>100000</v>
       </c>
       <c r="J104" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K104" s="44">
         <v>250000</v>
       </c>
       <c r="L104" s="44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M104" s="17">
         <v>750000</v>
@@ -7434,7 +7431,7 @@
         <v>1000</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G105" s="6">
         <v>2500</v>
@@ -7452,19 +7449,19 @@
         <v>10000</v>
       </c>
       <c r="L105" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M105" s="19">
         <v>80000</v>
       </c>
       <c r="N105" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O105" s="16">
         <v>240000</v>
       </c>
       <c r="P105" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q105" s="15">
         <v>700000</v>
@@ -7510,7 +7507,7 @@
         <v>1000</v>
       </c>
       <c r="F106" s="57" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G106" s="57">
         <v>2500</v>
@@ -7528,19 +7525,19 @@
         <v>10000</v>
       </c>
       <c r="L106" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M106" s="19">
         <v>80000</v>
       </c>
       <c r="N106" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O106" s="16">
         <v>240000</v>
       </c>
       <c r="P106" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q106" s="15">
         <v>700000</v>
@@ -7586,7 +7583,7 @@
         <v>1000</v>
       </c>
       <c r="F107" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G107" s="56">
         <v>2500</v>
@@ -7604,19 +7601,19 @@
         <v>10000</v>
       </c>
       <c r="L107" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M107" s="19">
         <v>80000</v>
       </c>
       <c r="N107" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O107" s="16">
         <v>240000</v>
       </c>
       <c r="P107" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q107" s="15">
         <v>700000</v>
@@ -7662,7 +7659,7 @@
         <v>1000</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G108" s="5">
         <v>2500</v>
@@ -7680,19 +7677,19 @@
         <v>10000</v>
       </c>
       <c r="L108" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M108" s="32">
         <v>80000</v>
       </c>
       <c r="N108" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O108" s="44">
         <v>240000</v>
       </c>
       <c r="P108" s="44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q108" s="17">
         <v>700000</v>
@@ -7897,7 +7894,7 @@
         <v>700</v>
       </c>
       <c r="H112" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I112" s="22">
         <v>1400</v>
@@ -7927,7 +7924,7 @@
         <v>28000</v>
       </c>
       <c r="R112" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S112" s="16">
         <v>56000</v>
@@ -7981,7 +7978,7 @@
         <v>700</v>
       </c>
       <c r="H113" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I113" s="22">
         <v>1400</v>
@@ -8011,7 +8008,7 @@
         <v>28000</v>
       </c>
       <c r="R113" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S113" s="16">
         <v>56000</v>
@@ -8065,7 +8062,7 @@
         <v>700</v>
       </c>
       <c r="H114" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I114" s="21">
         <v>1400</v>
@@ -8095,7 +8092,7 @@
         <v>28000</v>
       </c>
       <c r="R114" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S114" s="16">
         <v>56000</v>
@@ -8149,7 +8146,7 @@
         <v>700</v>
       </c>
       <c r="H115" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I115" s="23">
         <v>1400</v>
@@ -8179,7 +8176,7 @@
         <v>28000</v>
       </c>
       <c r="R115" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S115" s="16">
         <v>56000</v>
@@ -8233,7 +8230,7 @@
         <v>700</v>
       </c>
       <c r="H116" s="50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I116" s="50">
         <v>1400</v>
@@ -8263,7 +8260,7 @@
         <v>28000</v>
       </c>
       <c r="R116" s="52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S116" s="16">
         <v>56000</v>
@@ -8317,7 +8314,7 @@
         <v>700</v>
       </c>
       <c r="H117" s="76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I117" s="76">
         <v>1400</v>
@@ -8347,7 +8344,7 @@
         <v>28000</v>
       </c>
       <c r="R117" s="78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S117" s="55">
         <v>56000</v>
@@ -8401,7 +8398,7 @@
         <v>700</v>
       </c>
       <c r="H118" s="60" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I118" s="60">
         <v>1400</v>
@@ -8431,7 +8428,7 @@
         <v>28000</v>
       </c>
       <c r="R118" s="62" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S118" s="47">
         <v>56000</v>
@@ -8515,7 +8512,7 @@
         <v>50000</v>
       </c>
       <c r="R119" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S119" s="16">
         <v>100000</v>
@@ -8527,7 +8524,7 @@
         <v>250000</v>
       </c>
       <c r="V119" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W119" s="13">
         <v>500000</v>
@@ -8595,7 +8592,7 @@
         <v>50000</v>
       </c>
       <c r="R120" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S120" s="16">
         <v>100000</v>
@@ -8607,7 +8604,7 @@
         <v>250000</v>
       </c>
       <c r="V120" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W120" s="13">
         <v>500000</v>
@@ -8675,7 +8672,7 @@
         <v>50000</v>
       </c>
       <c r="R121" s="67" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S121" s="45">
         <v>100000</v>
@@ -8687,7 +8684,7 @@
         <v>250000</v>
       </c>
       <c r="V121" s="68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W121" s="69">
         <v>500000</v>
@@ -8755,7 +8752,7 @@
         <v>50000</v>
       </c>
       <c r="R122" s="72" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S122" s="46">
         <v>100000</v>
@@ -8767,7 +8764,7 @@
         <v>250000</v>
       </c>
       <c r="V122" s="73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W122" s="74">
         <v>500000</v>
@@ -8805,7 +8802,7 @@
         <v>700</v>
       </c>
       <c r="H123" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I123" s="22">
         <v>1400</v>
@@ -8835,7 +8832,7 @@
         <v>28000</v>
       </c>
       <c r="R123" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S123" s="16">
         <v>56000</v>
@@ -8889,7 +8886,7 @@
         <v>700</v>
       </c>
       <c r="H124" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I124" s="22">
         <v>1400</v>
@@ -8919,7 +8916,7 @@
         <v>28000</v>
       </c>
       <c r="R124" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S124" s="16">
         <v>56000</v>
@@ -8973,7 +8970,7 @@
         <v>700</v>
       </c>
       <c r="H125" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I125" s="21">
         <v>1400</v>
@@ -9003,7 +9000,7 @@
         <v>28000</v>
       </c>
       <c r="R125" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S125" s="16">
         <v>56000</v>
@@ -9057,7 +9054,7 @@
         <v>700</v>
       </c>
       <c r="H126" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I126" s="23">
         <v>1400</v>
@@ -9087,7 +9084,7 @@
         <v>28000</v>
       </c>
       <c r="R126" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S126" s="16">
         <v>56000</v>
@@ -9141,7 +9138,7 @@
         <v>700</v>
       </c>
       <c r="H127" s="50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I127" s="50">
         <v>1400</v>
@@ -9171,7 +9168,7 @@
         <v>28000</v>
       </c>
       <c r="R127" s="52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S127" s="16">
         <v>56000</v>
@@ -9225,7 +9222,7 @@
         <v>700</v>
       </c>
       <c r="H128" s="76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I128" s="76">
         <v>1400</v>
@@ -9255,7 +9252,7 @@
         <v>28000</v>
       </c>
       <c r="R128" s="78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S128" s="55">
         <v>56000</v>
@@ -9309,7 +9306,7 @@
         <v>700</v>
       </c>
       <c r="H129" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I129" s="28">
         <v>1400</v>
@@ -9339,7 +9336,7 @@
         <v>28000</v>
       </c>
       <c r="R129" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S129" s="47">
         <v>56000</v>
@@ -9423,7 +9420,7 @@
         <v>50000</v>
       </c>
       <c r="R130" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S130" s="16">
         <v>100000</v>
@@ -9435,7 +9432,7 @@
         <v>250000</v>
       </c>
       <c r="V130" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W130" s="13">
         <v>500000</v>
@@ -9503,7 +9500,7 @@
         <v>50000</v>
       </c>
       <c r="R131" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S131" s="16">
         <v>100000</v>
@@ -9515,7 +9512,7 @@
         <v>250000</v>
       </c>
       <c r="V131" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W131" s="13">
         <v>500000</v>
@@ -9583,7 +9580,7 @@
         <v>50000</v>
       </c>
       <c r="R132" s="67" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S132" s="45">
         <v>100000</v>
@@ -9595,7 +9592,7 @@
         <v>250000</v>
       </c>
       <c r="V132" s="68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W132" s="69">
         <v>500000</v>
@@ -9663,7 +9660,7 @@
         <v>50000</v>
       </c>
       <c r="R133" s="72" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S133" s="46">
         <v>100000</v>
@@ -9675,7 +9672,7 @@
         <v>250000</v>
       </c>
       <c r="V133" s="73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W133" s="74">
         <v>500000</v>
@@ -9701,7 +9698,7 @@
         <v>1000000</v>
       </c>
       <c r="D134" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E134" s="13">
         <v>1500000</v>
@@ -9761,7 +9758,7 @@
         <v>1000000</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E135" s="37">
         <v>1500000</v>
@@ -9821,7 +9818,7 @@
         <v>1000000</v>
       </c>
       <c r="D136" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E136" s="12">
         <v>1500000</v>
@@ -9881,7 +9878,7 @@
         <v>600000</v>
       </c>
       <c r="D137" s="79" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E137" s="13">
         <v>1200000</v>
@@ -9968,6 +9965,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
@@ -9975,12 +9978,6 @@
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="46" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>